<commit_message>
Fix cycles, first cut
</commit_message>
<xml_diff>
--- a/source_data/cycles_1_v2.xlsx
+++ b/source_data/cycles_1_v2.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EE97D5-6F69-EA4F-9B6B-BA6BE1B46BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460443E1-F976-644B-BA02-576B72114895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="10380" windowWidth="35800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="study" sheetId="2" r:id="rId1"/>
+    <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
+    <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
+    <sheet name="soa" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="75">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -50,9 +53,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Follow Up</t>
-  </si>
-  <si>
     <t>Cycle</t>
   </si>
   <si>
@@ -158,26 +158,119 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC:PE 1</t>
-  </si>
-  <si>
-    <t>BC:PE 2</t>
-  </si>
-  <si>
-    <t>BC:Weight</t>
-  </si>
-  <si>
-    <t>BC:Height</t>
-  </si>
-  <si>
     <t>BC/Profile</t>
+  </si>
+  <si>
+    <t>studyTitle</t>
+  </si>
+  <si>
+    <t>studyVersion</t>
+  </si>
+  <si>
+    <t>studyType</t>
+  </si>
+  <si>
+    <t>studyPhase</t>
+  </si>
+  <si>
+    <t>C98388=Interventional Study</t>
+  </si>
+  <si>
+    <t>C15602=Phase III Trial</t>
+  </si>
+  <si>
+    <t>Cycles Tests</t>
+  </si>
+  <si>
+    <t>organisationIdentifierScheme</t>
+  </si>
+  <si>
+    <t>organisationIdentifier</t>
+  </si>
+  <si>
+    <t>organisationName</t>
+  </si>
+  <si>
+    <t>organisationType</t>
+  </si>
+  <si>
+    <t>studyIdentifier</t>
+  </si>
+  <si>
+    <t>USGOV</t>
+  </si>
+  <si>
+    <t>CT-GOV</t>
+  </si>
+  <si>
+    <t>ClinicalTrials.gov</t>
+  </si>
+  <si>
+    <t>Registry</t>
+  </si>
+  <si>
+    <t>NCT12345678</t>
+  </si>
+  <si>
+    <t>therapeuticAreas</t>
+  </si>
+  <si>
+    <t>Not supported yet</t>
+  </si>
+  <si>
+    <t>studyDesignRationale</t>
+  </si>
+  <si>
+    <t>"Study design rationale put here"</t>
+  </si>
+  <si>
+    <t>studyDesignBlindingScheme</t>
+  </si>
+  <si>
+    <t>C49659=OPEN LABEL</t>
+  </si>
+  <si>
+    <t>trialIntentTypes</t>
+  </si>
+  <si>
+    <t>C15714=BASIC SCIENCE, C139174=DEVICE FEASIBILITY</t>
+  </si>
+  <si>
+    <t>trialTypes</t>
+  </si>
+  <si>
+    <t>C12345=Observational</t>
+  </si>
+  <si>
+    <t>interventionModel</t>
+  </si>
+  <si>
+    <t>C12346=None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screening </t>
+  </si>
+  <si>
+    <t>Follow-Up</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>BC: PE 1, BC: PE 2, BC: Weight, BC: Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,6 +282,29 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -251,6 +367,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,21 +704,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F975A6-8C40-A94B-B707-4567CE298AC4}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="4" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD730DE0-C074-8B4F-8463-AF26984F71A7}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B66121-AE3C-4E48-906B-C59A3DAEA708}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
     <col min="5" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
@@ -611,17 +1003,17 @@
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
@@ -636,513 +1028,381 @@
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>